<commit_message>
non-round and round trip distinction
</commit_message>
<xml_diff>
--- a/Data/Benchmark Lines/smalleuchalf.xlsx
+++ b/Data/Benchmark Lines/smalleuchalf.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC73FB48-3CC5-472B-AA39-B269B9BB4F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9470F7-0442-48DF-B82F-4AA5A308313E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1286,7 +1286,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>